<commit_message>
a flurry of work
</commit_message>
<xml_diff>
--- a/data/EAR_requirements_GBDgroups.xlsx
+++ b/data/EAR_requirements_GBDgroups.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARDIZED DATA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -251,12 +251,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="R1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Alon Shepon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+B12 in units of mcg/d
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>AGE GROUP</t>
   </si>
@@ -534,6 +557,25 @@
   <si>
     <t>as appeared in Table 4 in A Review of Dietary Zinc Recommendations, Gibson et al, Food and Nutrition Bulletin, Vol 37(4) 443-460, 2016</t>
   </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Institute of Medicine (US) Standing Committee on the Scientific Evaluation of Dietary Reference Intakes and its Panel on Folate, Other B Vitamins, and Choline. Dietary Reference Intakes for Thiamin, Riboflavin, Niacin, Vitamin B6, Folate, Vitamin B12, Pantothenic Acid, Biotin, and Choline. Washington (DC): National Academies Press (US); 1998. 9, Vitamin B12. Available from: https://www.ncbi.nlm.nih.gov/books/NBK114302/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(B12)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -542,7 +584,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -627,6 +669,32 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -649,7 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -675,6 +743,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1657,13 +1726,13 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="R47" sqref="R47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
@@ -1681,7 +1750,7 @@
     <col min="15" max="15" width="10.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1733,8 +1802,11 @@
       <c r="Q1" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1799,8 +1871,11 @@
         <f>AVERAGE(0.6,7.45)</f>
         <v>4.0250000000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1865,8 +1940,11 @@
         <f>AVERAGE(7.48,6.46)</f>
         <v>6.9700000000000006</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1931,8 +2009,11 @@
         <f>AVERAGE(9.35,12.14)</f>
         <v>10.745000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1994,8 +2075,11 @@
       <c r="Q5" s="4">
         <v>13.12</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2059,8 +2143,11 @@
         <f>Q5</f>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2124,8 +2211,11 @@
         <f t="shared" ref="Q7:Q22" si="1">Q6</f>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2189,8 +2279,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2254,8 +2347,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2319,8 +2415,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2384,8 +2483,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2449,8 +2551,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2514,8 +2619,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2579,8 +2687,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2644,8 +2755,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2709,8 +2823,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2774,8 +2891,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2839,8 +2959,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2904,8 +3027,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2969,8 +3095,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -3034,8 +3163,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3096,8 +3228,11 @@
         <f t="shared" si="1"/>
         <v>13.12</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3113,7 +3248,7 @@
       <c r="O23"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.8">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3129,7 +3264,7 @@
       <c r="O24"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.8">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3194,8 +3329,11 @@
         <f t="shared" si="2"/>
         <v>4.0250000000000004</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -3260,8 +3398,11 @@
         <f t="shared" si="3"/>
         <v>6.9700000000000006</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3326,8 +3467,11 @@
         <f>AVERAGE(7.95,10.32)</f>
         <v>9.1349999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R27">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -3389,8 +3533,11 @@
       <c r="Q28" s="4">
         <v>10.29</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R28" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -3455,8 +3602,11 @@
         <f>Q28</f>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3521,8 +3671,11 @@
         <f t="shared" ref="Q30:Q45" si="6">Q29</f>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -3587,8 +3740,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -3653,8 +3809,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -3719,8 +3878,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -3785,8 +3947,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -3851,8 +4016,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -3917,8 +4085,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -3983,8 +4154,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4049,8 +4223,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -4115,8 +4292,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4181,8 +4361,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -4247,8 +4430,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -4313,8 +4499,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -4379,8 +4568,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -4445,8 +4637,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -4508,8 +4703,11 @@
         <f t="shared" si="6"/>
         <v>10.29</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -4556,8 +4754,11 @@
         <f>[1]Protein!B12</f>
         <v>0.66</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.8">
+      <c r="R46">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.8">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -4603,6 +4804,9 @@
       <c r="M47" s="4">
         <f>[1]Protein!B12</f>
         <v>0.66</v>
+      </c>
+      <c r="R47">
+        <v>2.4</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.8">
@@ -4619,10 +4823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.8"/>
@@ -4672,6 +4876,11 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.8">
       <c r="A11" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.8">
+      <c r="A13" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>